<commit_message>
Scalar issue. Need to run all random distributions and MNIST
</commit_message>
<xml_diff>
--- a/PyTorch/PyTorch_experiments.xlsx
+++ b/PyTorch/PyTorch_experiments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\postCompletion\research\Accelerated-Blind-CNN-Descent-ABCD-\PyTorch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D02F389D-7F55-477B-98C1-0A6B839621B4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42DC219F-3ABF-4CC8-A761-2E5625C8CC59}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,39 +25,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
-  <si>
-    <t>Experiment</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Probability distribution</t>
   </si>
   <si>
-    <t>Layer by Layer</t>
-  </si>
-  <si>
     <t>CIFAR-10 test accuracy (%)</t>
   </si>
   <si>
     <t>MNIST test accuracy (%)</t>
-  </si>
-  <si>
-    <t>one</t>
-  </si>
-  <si>
-    <t>two</t>
-  </si>
-  <si>
-    <t>three</t>
-  </si>
-  <si>
-    <t>four</t>
-  </si>
-  <si>
-    <t>five</t>
-  </si>
-  <si>
-    <t>six</t>
   </si>
   <si>
     <t>Zero mean unit uniform</t>
@@ -393,22 +369,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -418,77 +390,20 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" t="b">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CIFAR10 complete; MNIST pending
</commit_message>
<xml_diff>
--- a/PyTorch/PyTorch_experiments.xlsx
+++ b/PyTorch/PyTorch_experiments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\postCompletion\research\Accelerated-Blind-CNN-Descent-ABCD-\PyTorch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42DC219F-3ABF-4CC8-A761-2E5625C8CC59}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0191D17F-2F61-4E35-8245-B32ED5F1D114}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -371,7 +371,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -395,15 +397,24 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
+      <c r="B2">
+        <v>9.9</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
+      <c r="B3">
+        <v>9.9600000000000009</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
+      </c>
+      <c r="B4">
+        <v>9.94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Batch experiments for normal distribution pending
</commit_message>
<xml_diff>
--- a/PyTorch/PyTorch_experiments.xlsx
+++ b/PyTorch/PyTorch_experiments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\postCompletion\research\Accelerated-Blind-CNN-Descent-ABCD-\PyTorch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0191D17F-2F61-4E35-8245-B32ED5F1D114}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DE07D1F-2B8A-48D0-964B-CB54E2A4FD5D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -398,7 +398,10 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>9.9</v>
+        <v>9.98</v>
+      </c>
+      <c r="C2">
+        <v>9.4600000000000009</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -406,7 +409,10 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>9.9600000000000009</v>
+        <v>9.86</v>
+      </c>
+      <c r="C3">
+        <v>75.069999999999993</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -414,7 +420,10 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>9.94</v>
+        <v>10.01</v>
+      </c>
+      <c r="C4">
+        <v>69.09</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Gradient check needs to be performed!
</commit_message>
<xml_diff>
--- a/PyTorch/PyTorch_experiments.xlsx
+++ b/PyTorch/PyTorch_experiments.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\postCompletion\research\Accelerated-Blind-CNN-Descent-ABCD-\PyTorch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DE07D1F-2B8A-48D0-964B-CB54E2A4FD5D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C24DCECD-7192-423C-9118-5AC625F4AA5F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Probability distribution</t>
   </si>
@@ -43,6 +44,15 @@
   </si>
   <si>
     <t>Normal</t>
+  </si>
+  <si>
+    <t>batch_size</t>
+  </si>
+  <si>
+    <t>MNIST (uniform) test accuracy (%)</t>
+  </si>
+  <si>
+    <t>MNIST (normal) test accuracy (%)</t>
   </si>
 </sst>
 </file>
@@ -371,7 +381,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -430,4 +440,102 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7635446E-E73F-4DC8-8904-E0F1111AC0A4}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>16</v>
+      </c>
+      <c r="B2">
+        <v>74.08</v>
+      </c>
+      <c r="C2">
+        <v>68.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>32</v>
+      </c>
+      <c r="B3">
+        <v>70.42</v>
+      </c>
+      <c r="C3">
+        <v>67.239999999999995</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>64</v>
+      </c>
+      <c r="B4">
+        <v>70.33</v>
+      </c>
+      <c r="C4">
+        <v>69.28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>128</v>
+      </c>
+      <c r="B5">
+        <v>72.790000000000006</v>
+      </c>
+      <c r="C5">
+        <v>74.61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>256</v>
+      </c>
+      <c r="B6">
+        <v>67.98</v>
+      </c>
+      <c r="C6">
+        <v>72.13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>512</v>
+      </c>
+      <c r="B7">
+        <v>74.739999999999995</v>
+      </c>
+      <c r="C7">
+        <v>67.59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>